<commit_message>
Xls file is loaded on server and poi works fine.
</commit_message>
<xml_diff>
--- a/xlsSectionsTestData/Sections.xlsx
+++ b/xlsSectionsTestData/Sections.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="24390" windowHeight="12840"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="24390" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Section1-8" sheetId="1" r:id="rId1"/>
+    <sheet name="Section809-812" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
   <si>
     <t>Section 1</t>
   </si>
@@ -188,6 +189,93 @@
   </si>
   <si>
     <t>geoCode26</t>
+  </si>
+  <si>
+    <t>Section 809</t>
+  </si>
+  <si>
+    <t>Section 810</t>
+  </si>
+  <si>
+    <t>geoCode27</t>
+  </si>
+  <si>
+    <t>geoCode28</t>
+  </si>
+  <si>
+    <t>geoCode29</t>
+  </si>
+  <si>
+    <t>geoCode30</t>
+  </si>
+  <si>
+    <t>geoCode31</t>
+  </si>
+  <si>
+    <t>Section 811</t>
+  </si>
+  <si>
+    <t>geoCode32</t>
+  </si>
+  <si>
+    <t>geoCode33</t>
+  </si>
+  <si>
+    <t>geoCode34</t>
+  </si>
+  <si>
+    <t>geoCode35</t>
+  </si>
+  <si>
+    <t>geoCode36</t>
+  </si>
+  <si>
+    <t>geoCode37</t>
+  </si>
+  <si>
+    <t>geoCode38</t>
+  </si>
+  <si>
+    <t>geoCode39</t>
+  </si>
+  <si>
+    <t>geoCode40</t>
+  </si>
+  <si>
+    <t>geoCode41</t>
+  </si>
+  <si>
+    <t>geoCode42</t>
+  </si>
+  <si>
+    <t>Section 812</t>
+  </si>
+  <si>
+    <t>geoCode43</t>
+  </si>
+  <si>
+    <t>geoCode44</t>
+  </si>
+  <si>
+    <t>geoCode45</t>
+  </si>
+  <si>
+    <t>geoCode46</t>
+  </si>
+  <si>
+    <t>geoCode47</t>
+  </si>
+  <si>
+    <t>geoCode48</t>
+  </si>
+  <si>
+    <t>geoCode49</t>
+  </si>
+  <si>
+    <t>geoCode50</t>
+  </si>
+  <si>
+    <t>geoCode51</t>
   </si>
 </sst>
 </file>
@@ -528,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -806,4 +894,275 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code optimization: * code is optimized in XlsFileParserService; * bug fixed in XlsFileParserService; + XlsFileParserInterface is added; * bug fixed in Section.
</commit_message>
<xml_diff>
--- a/xlsSectionsTestData/Sections.xlsx
+++ b/xlsSectionsTestData/Sections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="24390" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="24390" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Section1-8" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
-  <si>
-    <t>Section 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
   <si>
     <t>geo1</t>
   </si>
@@ -32,9 +29,6 @@
     <t>geoCode2</t>
   </si>
   <si>
-    <t>Section 2</t>
-  </si>
-  <si>
     <t>geo4</t>
   </si>
   <si>
@@ -53,9 +47,6 @@
     <t>geoCode6</t>
   </si>
   <si>
-    <t>Section 3</t>
-  </si>
-  <si>
     <t>geo7</t>
   </si>
   <si>
@@ -74,9 +65,6 @@
     <t>geoCode9</t>
   </si>
   <si>
-    <t>Section 4</t>
-  </si>
-  <si>
     <t>geo10</t>
   </si>
   <si>
@@ -95,9 +83,6 @@
     <t>geoCode12</t>
   </si>
   <si>
-    <t>Section 5</t>
-  </si>
-  <si>
     <t>geo13</t>
   </si>
   <si>
@@ -116,9 +101,6 @@
     <t>geoCode15</t>
   </si>
   <si>
-    <t>Section 6</t>
-  </si>
-  <si>
     <t>geo16</t>
   </si>
   <si>
@@ -137,9 +119,6 @@
     <t>geoCode18</t>
   </si>
   <si>
-    <t>Section 7</t>
-  </si>
-  <si>
     <t>geo19</t>
   </si>
   <si>
@@ -158,9 +137,6 @@
     <t>geoCode21</t>
   </si>
   <si>
-    <t>Section 8</t>
-  </si>
-  <si>
     <t>geo22</t>
   </si>
   <si>
@@ -276,6 +252,27 @@
   </si>
   <si>
     <t>geoCode51</t>
+  </si>
+  <si>
+    <t>Section 1123</t>
+  </si>
+  <si>
+    <t>Section 243</t>
+  </si>
+  <si>
+    <t>Section 365</t>
+  </si>
+  <si>
+    <t>Section 44</t>
+  </si>
+  <si>
+    <t>Section 544</t>
+  </si>
+  <si>
+    <t>Section 7908</t>
+  </si>
+  <si>
+    <t>Section 889087</t>
   </si>
 </sst>
 </file>
@@ -616,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -628,266 +625,266 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>33</v>
+      <c r="A18">
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -900,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -913,254 +910,254 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>